<commit_message>
Adds account email to Data Dictionary
</commit_message>
<xml_diff>
--- a/databases/WECAN data dictionary.xlsx
+++ b/databases/WECAN data dictionary.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="91">
   <si>
     <t>Data Type</t>
   </si>
@@ -283,6 +283,12 @@
   </si>
   <si>
     <t>Check if access was granted</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>User's email address (for password reset)</t>
   </si>
 </sst>
 </file>
@@ -520,6 +526,15 @@
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -529,14 +544,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -546,7 +553,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -848,10 +854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G76"/>
+  <dimension ref="A1:G77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,38 +872,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="15"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="16"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="12"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="4"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="13"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -915,12 +921,12 @@
       <c r="F4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -938,12 +944,12 @@
       <c r="F5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -961,12 +967,12 @@
       <c r="F6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -984,12 +990,12 @@
       <c r="F7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1007,13 +1013,13 @@
       <c r="F8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="3" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>9</v>
+      <c r="A9" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>12</v>
@@ -1030,111 +1036,111 @@
       <c r="F9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="1">
+        <v>255</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C11" s="5">
         <v>255</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="9" t="s">
+      <c r="F11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="12"/>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="12"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="9"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="9"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="13"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="1" t="s">
+      <c r="C15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G15" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
         <v>5</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="1">
-        <v>11</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>10</v>
@@ -1149,36 +1155,38 @@
         <v>14</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="1">
+        <v>11</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>22</v>
@@ -1193,209 +1201,207 @@
       <c r="F18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
+    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B20" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="8">
-        <v>11</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="8">
+      <c r="C20" s="5">
+        <v>11</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="5">
         <v>1</v>
       </c>
-      <c r="F19" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G19" s="9" t="s">
+      <c r="F20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="12"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="10"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="12"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="9"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="7"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="9"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="4"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="13"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="1" t="s">
+      <c r="C24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G23" s="6" t="s">
+      <c r="G24" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="16" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="1">
-        <v>11</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" s="1" t="s">
+      <c r="C25" s="1">
+        <v>11</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G24" s="6" t="s">
+      <c r="G25" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
+    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B26" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C26" s="5">
         <v>16</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D26" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" s="9" t="s">
+      <c r="F26" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="12"/>
-    </row>
-    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="10"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="12"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="9"/>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="7"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="9"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="4"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="13"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" s="1" t="s">
+      <c r="C30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G29" s="6" t="s">
+      <c r="G30" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="16" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
         <v>5</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" s="1">
-        <v>11</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>10</v>
@@ -1410,38 +1416,38 @@
         <v>14</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G31" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="1">
+        <v>11</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C32" s="1">
-        <v>255</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>12</v>
@@ -1458,276 +1464,276 @@
       <c r="F33" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G33" s="6" t="s">
+      <c r="G33" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="1">
+        <v>255</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C34" s="1">
-        <v>11</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G34" s="6" t="s">
+      <c r="C35" s="1">
+        <v>11</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G35" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="7" t="s">
+    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B36" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="8">
+      <c r="C36" s="5">
         <v>1</v>
       </c>
-      <c r="D35" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E35" s="8">
+      <c r="D36" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" s="5">
         <v>1</v>
       </c>
-      <c r="F35" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G35" s="9" t="s">
+      <c r="F36" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="10"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="12"/>
-    </row>
-    <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="10"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="12"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="7"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="9"/>
+    </row>
+    <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="7"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="9"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="4"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="13"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D39" s="1" t="s">
+      <c r="C40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="F40" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G39" s="6" t="s">
+      <c r="G40" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="16" t="s">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C40" s="1">
-        <v>11</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F40" s="1" t="s">
+      <c r="C41" s="1">
+        <v>11</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G40" s="6" t="s">
+      <c r="G41" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="7" t="s">
+    <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="B42" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C41" s="8">
+      <c r="C42" s="5">
         <v>2</v>
       </c>
-      <c r="D41" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E41" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F41" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G41" s="9" t="s">
+      <c r="D42" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="10"/>
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="12"/>
-    </row>
-    <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="10"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="12"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="7"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="9"/>
+    </row>
+    <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="7"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="9"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="4"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="13"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D45" s="1" t="s">
+      <c r="C46" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G45" s="6" t="s">
+      <c r="G46" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="16" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C46" s="1">
-        <v>11</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F46" s="1" t="s">
+      <c r="C47" s="1">
+        <v>11</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F47" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G46" s="6" t="s">
+      <c r="G47" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G47" s="6" t="s">
+      <c r="C48" s="1"/>
+      <c r="D48" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G48" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C48" s="1">
-        <v>11</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G48" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
-        <v>55</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>10</v>
@@ -1744,140 +1750,140 @@
       <c r="F49" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G49" s="6" t="s">
+      <c r="G49" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50" s="1">
+        <v>11</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G50" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="7" t="s">
+    <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="B51" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C50" s="8">
-        <v>11</v>
-      </c>
-      <c r="D50" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E50" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F50" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G50" s="9" t="s">
+      <c r="C51" s="5">
+        <v>11</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G51" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="10"/>
-      <c r="B51" s="11"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="12"/>
-    </row>
-    <row r="52" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="10"/>
-      <c r="B52" s="11"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
-      <c r="G52" s="12"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="7"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="9"/>
+    </row>
+    <row r="53" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="7"/>
+      <c r="B53" s="8"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="9"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="4"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
+      <c r="B54" s="12"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="13"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B55" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D54" s="1" t="s">
+      <c r="C55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="E55" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F54" s="1" t="s">
+      <c r="F55" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G54" s="6" t="s">
+      <c r="G55" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="16" t="s">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B56" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C55" s="1">
-        <v>11</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F55" s="1" t="s">
+      <c r="C56" s="1">
+        <v>11</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G55" s="6" t="s">
+      <c r="G56" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C56" s="1">
-        <v>128</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G56" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
-        <v>63</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C57" s="1">
-        <v>255</v>
+        <v>128</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>13</v>
@@ -1888,42 +1894,42 @@
       <c r="F57" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G57" s="6" t="s">
-        <v>68</v>
+      <c r="G57" s="3" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
-        <v>64</v>
+      <c r="A58" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C58" s="1">
-        <v>8</v>
+        <v>255</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G58" s="6" t="s">
-        <v>85</v>
+      <c r="G58" s="3" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="5" t="s">
-        <v>65</v>
+      <c r="A59" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C59" s="1">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>15</v>
@@ -1934,232 +1940,232 @@
       <c r="F59" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G59" s="6" t="s">
+      <c r="G59" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C60" s="1">
+        <v>64</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G60" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="7" t="s">
+    <row r="61" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B60" s="8" t="s">
+      <c r="B61" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C60" s="8">
+      <c r="C61" s="5">
         <v>1</v>
       </c>
-      <c r="D60" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E60" s="8">
+      <c r="D61" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E61" s="5">
         <v>0</v>
       </c>
-      <c r="F60" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G60" s="9" t="s">
+      <c r="F61" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G61" s="6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="10"/>
-      <c r="B61" s="11"/>
-      <c r="C61" s="11"/>
-      <c r="D61" s="11"/>
-      <c r="E61" s="11"/>
-      <c r="F61" s="11"/>
-      <c r="G61" s="12"/>
-    </row>
-    <row r="62" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="10"/>
-      <c r="B62" s="11"/>
-      <c r="C62" s="11"/>
-      <c r="D62" s="11"/>
-      <c r="E62" s="11"/>
-      <c r="F62" s="11"/>
-      <c r="G62" s="12"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="7"/>
+      <c r="B62" s="8"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="8"/>
+      <c r="E62" s="8"/>
+      <c r="F62" s="8"/>
+      <c r="G62" s="9"/>
+    </row>
+    <row r="63" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="7"/>
+      <c r="B63" s="8"/>
+      <c r="C63" s="8"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="8"/>
+      <c r="G63" s="9"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-      <c r="G63" s="4"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="5" t="s">
+      <c r="B64" s="12"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="12"/>
+      <c r="F64" s="12"/>
+      <c r="G64" s="13"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D64" s="1" t="s">
+      <c r="C65" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E64" s="1" t="s">
+      <c r="E65" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F64" s="1" t="s">
+      <c r="F65" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G64" s="6" t="s">
+      <c r="G65" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="16" t="s">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C65" s="1">
-        <v>11</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F65" s="1" t="s">
+      <c r="C66" s="1">
+        <v>11</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F66" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G65" s="6" t="s">
+      <c r="G66" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B67" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C67" s="1">
         <v>255</v>
       </c>
-      <c r="D66" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G66" s="6" t="s">
+      <c r="D67" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G67" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="7" t="s">
+    <row r="68" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B67" s="8" t="s">
+      <c r="B68" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C67" s="8">
+      <c r="C68" s="5">
         <v>255</v>
       </c>
-      <c r="D67" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E67" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F67" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G67" s="9" t="s">
+      <c r="D68" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G68" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="10"/>
-      <c r="B68" s="11"/>
-      <c r="C68" s="11"/>
-      <c r="D68" s="11"/>
-      <c r="E68" s="11"/>
-      <c r="F68" s="11"/>
-      <c r="G68" s="12"/>
-    </row>
-    <row r="69" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="10"/>
-      <c r="B69" s="11"/>
-      <c r="C69" s="11"/>
-      <c r="D69" s="11"/>
-      <c r="E69" s="11"/>
-      <c r="F69" s="11"/>
-      <c r="G69" s="12"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="7"/>
+      <c r="B69" s="8"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8"/>
+      <c r="E69" s="8"/>
+      <c r="F69" s="8"/>
+      <c r="G69" s="9"/>
+    </row>
+    <row r="70" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="7"/>
+      <c r="B70" s="8"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8"/>
+      <c r="E70" s="8"/>
+      <c r="F70" s="8"/>
+      <c r="G70" s="9"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
-      <c r="E70" s="3"/>
-      <c r="F70" s="3"/>
-      <c r="G70" s="4"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
+      <c r="B71" s="12"/>
+      <c r="C71" s="12"/>
+      <c r="D71" s="12"/>
+      <c r="E71" s="12"/>
+      <c r="F71" s="12"/>
+      <c r="G71" s="13"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B72" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C71" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D71" s="1" t="s">
+      <c r="C72" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E71" s="1" t="s">
+      <c r="E72" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F71" s="1" t="s">
+      <c r="F72" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G71" s="6" t="s">
+      <c r="G72" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="16" t="s">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="10" t="s">
         <v>5</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C72" s="1">
-        <v>11</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G72" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
-        <v>76</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>10</v>
@@ -2174,15 +2180,15 @@
         <v>14</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G73" s="6" t="s">
-        <v>79</v>
+        <v>15</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="5" t="s">
-        <v>54</v>
+      <c r="A74" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>10</v>
@@ -2199,66 +2205,89 @@
       <c r="F74" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G74" s="6" t="s">
+      <c r="G74" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C75" s="1">
+        <v>11</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G75" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="5" t="s">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B76" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C75" s="1"/>
-      <c r="D75" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G75" s="6" t="s">
+      <c r="C76" s="1"/>
+      <c r="D76" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G76" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="7" t="s">
+    <row r="77" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B76" s="8" t="s">
+      <c r="B77" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C76" s="8">
+      <c r="C77" s="5">
         <v>1</v>
       </c>
-      <c r="D76" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E76" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F76" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G76" s="9" t="s">
+      <c r="D77" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G77" s="6" t="s">
         <v>88</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A53:G53"/>
-    <mergeCell ref="A63:G63"/>
-    <mergeCell ref="A70:G70"/>
+    <mergeCell ref="A54:G54"/>
+    <mergeCell ref="A64:G64"/>
+    <mergeCell ref="A71:G71"/>
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A13:G13"/>
-    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="A23:G23"/>
     <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="A38:G38"/>
-    <mergeCell ref="A44:G44"/>
+    <mergeCell ref="A29:G29"/>
+    <mergeCell ref="A39:G39"/>
+    <mergeCell ref="A45:G45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>